<commit_message>
updates to alt text for griafe() plots
</commit_message>
<xml_diff>
--- a/ges_health_study_app/text_dictionary.xlsx
+++ b/ges_health_study_app/text_dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sheenamartenies/Library/CloudStorage/Box-Box/Research/Projects/ges_health_study_app/ges_health_study_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB95A40-6023-0F41-8BF1-A25506BC4978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7496217B-8204-494F-8671-3F074E091E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28400" windowHeight="16320" xr2:uid="{8CCB3879-A5FF-D846-9F66-5161AE062B3F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="348">
   <si>
     <t>text_id</t>
   </si>
@@ -1076,6 +1076,12 @@
   </si>
   <si>
     <t>Scroll over each neighborhood to find its name.</t>
+  </si>
+  <si>
+    <t>An interactive map showing the names of Denver neighborhoods.</t>
+  </si>
+  <si>
+    <t>Un mapa interactivo que muestra los nombres de los vecindarios de Denver.</t>
   </si>
 </sst>
 </file>
@@ -1488,8 +1494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{548E5ED1-4340-C04D-8029-23B2D57DC5C7}">
   <dimension ref="A1:C117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" zoomScale="92" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B101" sqref="B101"/>
+    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="92" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C117" sqref="C117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2776,9 +2782,15 @@
         <v>340</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>327</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>347</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding the geocoding feature to get neighborhoods for addresses
</commit_message>
<xml_diff>
--- a/ges_health_study_app/text_dictionary.xlsx
+++ b/ges_health_study_app/text_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sheenamartenies/Library/CloudStorage/Box-Box/Research/Projects/ges_health_study_app/ges_health_study_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7496217B-8204-494F-8671-3F074E091E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72932464-8EEE-D946-95A8-DB8ACE469CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28400" windowHeight="16320" xr2:uid="{8CCB3879-A5FF-D846-9F66-5161AE062B3F}"/>
+    <workbookView xWindow="-34780" yWindow="1200" windowWidth="28400" windowHeight="16320" xr2:uid="{8CCB3879-A5FF-D846-9F66-5161AE062B3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="361">
   <si>
     <t>text_id</t>
   </si>
@@ -1082,6 +1082,45 @@
   </si>
   <si>
     <t>Un mapa interactivo que muestra los nombres de los vecindarios de Denver.</t>
+  </si>
+  <si>
+    <t>text_115</t>
+  </si>
+  <si>
+    <t>text_116</t>
+  </si>
+  <si>
+    <t>text_117</t>
+  </si>
+  <si>
+    <t>text_118</t>
+  </si>
+  <si>
+    <t>text_119</t>
+  </si>
+  <si>
+    <t>Find a Neighborhood</t>
+  </si>
+  <si>
+    <t>Enter an address to find its neighborhood:</t>
+  </si>
+  <si>
+    <t>Format: 213 Anystreet, Denver, CO 80216</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Encuentra un vecindario</t>
+  </si>
+  <si>
+    <t>Introduzca una dirección para encontrar su barrio:</t>
+  </si>
+  <si>
+    <t>Formato: 213 Anystreet, Denver, CO 80216</t>
+  </si>
+  <si>
+    <t>Dirección</t>
   </si>
 </sst>
 </file>
@@ -1492,10 +1531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{548E5ED1-4340-C04D-8029-23B2D57DC5C7}">
-  <dimension ref="A1:C117"/>
+  <dimension ref="A1:C122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="92" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C117" sqref="C117"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="92" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A123" sqref="A123:XFD124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2793,6 +2832,61 @@
         <v>347</v>
       </c>
     </row>
+    <row r="118" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A118" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A119" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A120" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A121" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A122" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updating readme; updating gitignore; error handling in "find a neighborhood", adding development code for reproducibility, updates to text_dictionary
</commit_message>
<xml_diff>
--- a/ges_health_study_app/text_dictionary.xlsx
+++ b/ges_health_study_app/text_dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sheenamartenies/Library/CloudStorage/Box-Box/Research/Projects/ges_health_study_app/ges_health_study_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72932464-8EEE-D946-95A8-DB8ACE469CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96D7602-9DC0-FA40-9912-79D9ABAE3414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-34780" yWindow="1200" windowWidth="28400" windowHeight="16320" xr2:uid="{8CCB3879-A5FF-D846-9F66-5161AE062B3F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="373">
   <si>
     <t>text_id</t>
   </si>
@@ -1108,9 +1108,6 @@
     <t>Format: 213 Anystreet, Denver, CO 80216</t>
   </si>
   <si>
-    <t>Address</t>
-  </si>
-  <si>
     <t>Encuentra un vecindario</t>
   </si>
   <si>
@@ -1120,7 +1117,46 @@
     <t>Formato: 213 Anystreet, Denver, CO 80216</t>
   </si>
   <si>
-    <t>Dirección</t>
+    <t>text_120</t>
+  </si>
+  <si>
+    <t>text_121</t>
+  </si>
+  <si>
+    <t>text_122</t>
+  </si>
+  <si>
+    <t>text_123</t>
+  </si>
+  <si>
+    <t>About the "Find a Neighborhood" tool:</t>
+  </si>
+  <si>
+    <t>"When you submit a geocode request, the web server automatically collects certain technical information from your computer and about your connection. The only information that is stored is IP Address (for batch and single address submissions) and submitted address (only for single address submissions). The information is stored on a server, which is internal to the Census network.  This server is only accessible by Census Bureau staff, who are bound by the confidentiality requirements set forth in Title 13 of the United States Code and requires multiple levels of approval. This information is only used to monitor and track the performance of the Geocoder."</t>
+  </si>
+  <si>
+    <t>To find the neighborhood associated with an address, we use a geocoder run by the US Census Bureau. The following information from the US Census Bureau descibes how they use the address information you provide:</t>
+  </si>
+  <si>
+    <t>Acerca de la herramienta "Buscar un vecindario":</t>
+  </si>
+  <si>
+    <t>Para encontrar el vecindario asociado con una dirección, utilizamos un geocodificador administrado por la Oficina del Censo de los EE. UU. La siguiente información de la Oficina del Censo de los EE. UU. describe cómo utilizan la información de la dirección que usted proporciona:</t>
+  </si>
+  <si>
+    <t>"Cuando envía una solicitud de geocodificación, el servidor web recopila automáticamente cierta información técnica de su computadora y sobre su conexión. La única información que se almacena es la dirección IP (para envíos por lotes y de una sola dirección) y la dirección enviada (solo para envíos de una sola dirección). La información se almacena en un servidor, que es interno a la red del Censo. A este servidor solo puede acceder el personal de la Oficina del Censo, que está sujeto a los requisitos de confidencialidad establecidos en el Título 13 del Código de los Estados Unidos y requiere múltiples niveles de aprobación. Esta información solo se utiliza para monitorear y hacer un seguimiento del rendimiento del geocodificador".</t>
+  </si>
+  <si>
+    <t>Si no desea ingresar su propia dirección, puede ingresar la dirección de una empresa local u otra ubicación en el vecindario de interés.</t>
+  </si>
+  <si>
+    <t>If you do not wish to enter your own address, you can enter the address of a local business or another location in the neighborhood of interest.</t>
+  </si>
+  <si>
+    <t>Dirección:</t>
+  </si>
+  <si>
+    <t>Address:</t>
   </si>
 </sst>
 </file>
@@ -1531,10 +1567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{548E5ED1-4340-C04D-8029-23B2D57DC5C7}">
-  <dimension ref="A1:C122"/>
+  <dimension ref="A1:C126"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A109" zoomScale="92" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A123" sqref="A123:XFD124"/>
+      <selection activeCell="C130" sqref="C130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2840,7 +2876,7 @@
         <v>353</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2851,7 +2887,7 @@
         <v>354</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2862,7 +2898,7 @@
         <v>355</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2870,10 +2906,10 @@
         <v>351</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>356</v>
+        <v>372</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>360</v>
+        <v>371</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2884,7 +2920,51 @@
         <v>353</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A123" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A124" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="136" x14ac:dyDescent="0.2">
+      <c r="A125" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A126" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>369</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to text dictionary
</commit_message>
<xml_diff>
--- a/ges_health_study_app/text_dictionary.xlsx
+++ b/ges_health_study_app/text_dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sheenamartenies/Library/CloudStorage/Box-Box/Research/Projects/ges_health_study_app/ges_health_study_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96D7602-9DC0-FA40-9912-79D9ABAE3414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F603D1-5399-F945-BFDC-085860A0533B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-34780" yWindow="1200" windowWidth="28400" windowHeight="16320" xr2:uid="{8CCB3879-A5FF-D846-9F66-5161AE062B3F}"/>
   </bookViews>
@@ -769,12 +769,6 @@
     <t>text_86</t>
   </si>
   <si>
-    <t>The data and code used to develop this Shiny app can be found on Github: &lt;a href='https://github.com/smartenies/ges_health_study_app'&gt; GES Health Study App&lt;/a&gt;.</t>
-  </si>
-  <si>
-    <t>Los datos y el código utilizados para desarrollar esta aplicación Shiny se pueden encontrar en Github: &lt;a href='https://github.com/smartenies/ges_health_study_app'&gt;Aplicación de estudio de salud GES&lt;/a&gt;.</t>
-  </si>
-  <si>
     <t>Puede encontrar información sobre el trabajo que realiza el CDPHE para proteger la salud y el medio ambiente en el &lt;a href='https://cdphe.colorado.gov/public-information'&gt;sitio web de información pública del CDPHE&lt;/a&gt;.</t>
   </si>
   <si>
@@ -1157,6 +1151,12 @@
   </si>
   <si>
     <t>Address:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The code and methods used to develop this Shiny app can be found on Github: &lt;a href='https://github.com/smartenies/ges_health_study_app'&gt; GES Health Study App&lt;/a&gt;. </t>
+  </si>
+  <si>
+    <t>El código y los métodos utilizados para desarrollar esta aplicación Shiny se pueden encontrar en Github: &lt;a href='https://github.com/smartenies/ges_health_study_app'&gt;Aplicación de estudio de salud GES&lt;/a&gt;.</t>
   </si>
 </sst>
 </file>
@@ -1569,8 +1569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{548E5ED1-4340-C04D-8029-23B2D57DC5C7}">
   <dimension ref="A1:C126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="92" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C130" sqref="C130"/>
+    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="92" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1605,13 +1605,13 @@
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>249</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1674,10 +1674,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1710,7 +1710,7 @@
         <v>47</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1718,10 +1718,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="85" x14ac:dyDescent="0.2">
@@ -1729,10 +1729,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1765,7 +1765,7 @@
         <v>61</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1787,7 +1787,7 @@
         <v>63</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1809,7 +1809,7 @@
         <v>65</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1831,7 +1831,7 @@
         <v>181</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1861,7 +1861,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>184</v>
@@ -1949,7 +1949,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>192</v>
@@ -2202,7 +2202,7 @@
         <v>98</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>214</v>
@@ -2301,10 +2301,10 @@
         <v>107</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -2312,10 +2312,10 @@
         <v>108</v>
       </c>
       <c r="B67" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="C67" s="4" t="s">
         <v>246</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2554,62 +2554,62 @@
         <v>242</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>243</v>
+        <v>371</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>244</v>
+        <v>372</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C90" s="2" t="s">
         <v>260</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>192</v>
@@ -2617,354 +2617,354 @@
     </row>
     <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B124" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="C124" s="2" t="s">
         <v>365</v>
-      </c>
-      <c r="C124" s="2" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="136" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor edits, CC resources added
</commit_message>
<xml_diff>
--- a/ges_health_study_app/text_dictionary.xlsx
+++ b/ges_health_study_app/text_dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sheenamartenies/Library/CloudStorage/Box-Box/Research/Projects/ges_health_study_app/ges_health_study_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09155EF1-ACA2-DD4D-B9E5-C62B0745994C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9958B47-6550-404A-AAB9-42AC83FEAF0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16320" xr2:uid="{8CCB3879-A5FF-D846-9F66-5161AE062B3F}"/>
+    <workbookView xWindow="-34960" yWindow="2580" windowWidth="28800" windowHeight="16320" xr2:uid="{8CCB3879-A5FF-D846-9F66-5161AE062B3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="373">
   <si>
     <t>text_id</t>
   </si>
@@ -263,9 +263,6 @@
     <t>Save a CSV file</t>
   </si>
   <si>
-    <t>On this page, you can visualize maps of population variables and important environmental variables at the neighborhood level. To get started, choose a population variable and an environmental variable from the menu on the left-hand side of this page (Map Options).</t>
-  </si>
-  <si>
     <t>Under these maps are two charts (Variable Distributions) showing the range of values measured for each of your selected variables.</t>
   </si>
   <si>
@@ -437,15 +434,6 @@
     <t>Resources to Learn More</t>
   </si>
   <si>
-    <t>To learn more about health and environment in Globeville, Elyria, and Swansea, check out these other great resources:</t>
-  </si>
-  <si>
-    <t>Resource 3</t>
-  </si>
-  <si>
-    <t>Resource 4</t>
-  </si>
-  <si>
     <t>This dynamic mapping tool is a collaboration between ENVIRONS and the GES Health Study Community Council. This tool allows users to compare population characteristics and environmental exposures across neighborhoods in Denver. It was built with community data needs in mind and informed by feedback from our GES Community Council.</t>
   </si>
   <si>
@@ -609,9 +597,6 @@
   </si>
   <si>
     <t>Guardar un archivo CSV</t>
-  </si>
-  <si>
-    <t>En esta página, puede visualizar mapas de variables de población y variables ambientales importantes a nivel de barrio. Para comenzar, elija una variable de población y una variable ambiental en el menú del lado izquierdo de esta página (Opciones de mapa).</t>
   </si>
   <si>
     <t>A continuación aparecerán mapas de vecindarios que muestran estas dos variables para cada uno de los vecindarios de Denver.</t>
@@ -706,15 +691,6 @@
     <t>Recursos para aprender más</t>
   </si>
   <si>
-    <t>Para obtener más información sobre la salud y el medio ambiente en Globeville, Elyria y Swansea, consulte estos otros excelentes recursos:</t>
-  </si>
-  <si>
-    <t>Recurso 3</t>
-  </si>
-  <si>
-    <t>Recurso 4</t>
-  </si>
-  <si>
     <t>Esta herramienta de mapeo dinámico es una colaboración entre ENVIRONS y el Consejo Comunitario del Estudio de Salud de GES. Esta herramienta permite a los usuarios comparar las características de la población y las exposiciones ambientales en los vecindarios de Denver. Se creó teniendo en cuenta las necesidades de datos de la comunidad y se basó en los comentarios de nuestro Consejo Comunitario de GES.</t>
   </si>
   <si>
@@ -763,18 +739,6 @@
     <t>text_86</t>
   </si>
   <si>
-    <t>Puede encontrar información sobre el trabajo que realiza el CDPHE para proteger la salud y el medio ambiente en el &lt;a href='https://cdphe.colorado.gov/public-information'&gt;sitio web de información pública del CDPHE&lt;/a&gt;.</t>
-  </si>
-  <si>
-    <t>To learn more about environmental justice issues across Colorado, check out  &lt;a href='https://cdphe.colorado.gov/enviroscreen'&gt; Colorado Enviroscreen 2.0&lt;/a&gt;.</t>
-  </si>
-  <si>
-    <t>Information about the work the CDPHE does to protect health and environment can be found on the &lt;a href='https://cdphe.colorado.gov/public-information'&gt;CDPHE Public Information website&lt;/a&gt;.</t>
-  </si>
-  <si>
-    <t>Para obtener más información sobre cuestiones de justicia ambiental en Colorado, consulte &lt;a href='https://cdphe.colorado.gov/enviroscreen'&gt; Colorado Enviroscreen 2.0&lt;/a&gt;.</t>
-  </si>
-  <si>
     <t>text_access</t>
   </si>
   <si>
@@ -871,12 +835,6 @@
     <t>Fuente de datos: Denver Open Data</t>
   </si>
   <si>
-    <t>On this page, you can visualize maps of population variables and important health variables at the neighborhood level. To get started, choose a population variable and health outcome variable from the menu on the left-hand side of this page (Map Options).</t>
-  </si>
-  <si>
-    <t>En esta página, puede visualizar mapas de variables de población y variables de salud importantes a nivel de barrio. Para comenzar, elija una variable de población y una variable de resultado de salud en el menú del lado izquierdo de esta página (Opciones de mapa).</t>
-  </si>
-  <si>
     <t>Desplácese sobre cada barrio para encontrar su nombre.</t>
   </si>
   <si>
@@ -1157,6 +1115,48 @@
   </si>
   <si>
     <t>Los miembros actuales del Consejo Comunitario de GES que contribuyeron al desarrollo de esta herramienta son Nancy Santos (residente de Swansea), Dolores Alfaro (residente de Elyria), Ana Varela (residente de Elyria), y Sandra Ruiz Parrilla (residente de Globeville). Los ex miembros del Consejo Comunitario de GES que contribuyeron a la interpretación de los datos comunitarios incluidos en esta herramienta incluyen a Maria de Santiago y Rebecca Trujillo.</t>
+  </si>
+  <si>
+    <t>On this page, you can visualize maps of population variables and important environmental variables at the neighborhood level. To get started, choose a population variable and an environmental variable from the menu on the left-hand side of this page (top of the page on mobile) (Map Options).</t>
+  </si>
+  <si>
+    <t>On this page, you can visualize maps of population variables and important health variables at the neighborhood level. To get started, choose a population variable and health outcome variable from the menu on the left-hand side of this page  (top of the page on mobile)  (Map Options).</t>
+  </si>
+  <si>
+    <t>En esta página, puede visualizar mapas de variables de población y variables de salud importantes a nivel de barrio. Para comenzar, elija una variable de población y una variable de resultado de salud en el menú del lado izquierdo de esta página (parte superior de la página en el móvil) (Opciones de mapa).</t>
+  </si>
+  <si>
+    <t>En esta página, puede visualizar mapas de variables de población y variables ambientales importantes a nivel de barrio. Para comenzar, elija una variable de población y una variable ambiental en el menú del lado izquierdo de esta página (parte superior de la página en el móvil) (Opciones de mapa).</t>
+  </si>
+  <si>
+    <t>text_124</t>
+  </si>
+  <si>
+    <t>text_125</t>
+  </si>
+  <si>
+    <t>To learn more about efforts to promote health, environment, food, and climate justice in Globeville, Elyria, and Swansea, check out these other great organizations:</t>
+  </si>
+  <si>
+    <t>Para obtener más información sobre los esfuerzos para promover la salud, el medio ambiente, la alimentación y la justicia climática en Globeville, Elyria y Swansea, consulte estas otras excelentes organizaciones:</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.ges-coalition.org/'&gt;GES Coalition&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.greenhouseconnectioncenter.com/'&gt;Green House Connection Center&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.facebook.com/p/Elyria-Globeville-Swansea-Partners-100083009972208/'&gt;EGS and Partners&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.cultivando.org/'&gt;Cultivando&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.birdseedcollective.org/'&gt;Birdseed Collective&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://groundworkcolorado.org/'&gt;Groundwork Denver&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -1180,16 +1180,19 @@
     <font>
       <sz val="12"/>
       <name val="Aptos"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF222222"/>
       <name val="Aptos"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF1F1F1F"/>
       <name val="Aptos"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1567,10 +1570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{548E5ED1-4340-C04D-8029-23B2D57DC5C7}">
-  <dimension ref="A1:C126"/>
+  <dimension ref="A1:C128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="92" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="92" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1597,7 +1600,7 @@
         <v>51</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>60</v>
@@ -1605,13 +1608,13 @@
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1630,10 +1633,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1674,10 +1677,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1710,7 +1713,7 @@
         <v>47</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1718,10 +1721,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="85" x14ac:dyDescent="0.2">
@@ -1729,10 +1732,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1765,7 +1768,7 @@
         <v>61</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1776,7 +1779,7 @@
         <v>62</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -1787,7 +1790,7 @@
         <v>63</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1798,7 +1801,7 @@
         <v>64</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1809,7 +1812,7 @@
         <v>65</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1820,7 +1823,7 @@
         <v>66</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1828,10 +1831,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1842,7 +1845,7 @@
         <v>67</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1853,7 +1856,7 @@
         <v>68</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1861,10 +1864,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>339</v>
+        <v>325</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1875,7 +1878,7 @@
         <v>69</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1886,7 +1889,7 @@
         <v>70</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1897,7 +1900,7 @@
         <v>71</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1908,7 +1911,7 @@
         <v>72</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1919,7 +1922,7 @@
         <v>73</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1930,18 +1933,18 @@
         <v>74</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>75</v>
+        <v>359</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>191</v>
+        <v>362</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1949,10 +1952,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1960,10 +1963,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -1971,10 +1974,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -1982,10 +1985,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1993,10 +1996,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2004,10 +2007,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2015,10 +2018,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2026,10 +2029,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2037,934 +2040,956 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="119" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="187" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B65" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
+      <c r="B66" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B66" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
+      <c r="B67" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B67" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>134</v>
+      <c r="B68" s="2" t="s">
+        <v>369</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>223</v>
+        <v>369</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>135</v>
+        <v>109</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>370</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>224</v>
+        <v>370</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>371</v>
+        <v>357</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B80" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C80" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B81" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C81" s="2" t="s">
         <v>155</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B82" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C82" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C86" s="2" t="s">
         <v>168</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B87" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C87" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>368</v>
+        <v>354</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>369</v>
+        <v>355</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>277</v>
+        <v>360</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>278</v>
+        <v>361</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C95" s="2" t="s">
         <v>265</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B96" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="B96" s="2" t="s">
-        <v>280</v>
-      </c>
       <c r="C96" s="2" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B97" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="B97" s="2" t="s">
-        <v>281</v>
-      </c>
       <c r="C97" s="2" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B98" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="B98" s="2" t="s">
-        <v>282</v>
-      </c>
       <c r="C98" s="2" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>292</v>
+        <v>278</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>307</v>
+        <v>293</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>308</v>
+        <v>294</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>302</v>
+        <v>288</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>306</v>
+        <v>292</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>312</v>
+        <v>298</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>325</v>
+        <v>311</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>326</v>
+        <v>312</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>337</v>
+        <v>323</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C112" s="2" t="s">
         <v>318</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C113" s="2" t="s">
         <v>319</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C114" s="2" t="s">
         <v>320</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C115" s="2" t="s">
         <v>321</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="C116" s="2" t="s">
         <v>322</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="C116" s="2" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>343</v>
+        <v>329</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>344</v>
+        <v>330</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>352</v>
+        <v>338</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>350</v>
+        <v>336</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>353</v>
+        <v>339</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>351</v>
+        <v>337</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>354</v>
+        <v>340</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>367</v>
+        <v>353</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>366</v>
+        <v>352</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>352</v>
+        <v>338</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>355</v>
+        <v>341</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>359</v>
+        <v>345</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>370</v>
+        <v>356</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>356</v>
+        <v>342</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>361</v>
+        <v>347</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>362</v>
+        <v>348</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="136" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>357</v>
+        <v>343</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>363</v>
+        <v>349</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>358</v>
+        <v>344</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
       <c r="C126" s="2" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A127" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A128" s="1" t="s">
         <v>364</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>372</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrections to text dictionary; clarification in readme
</commit_message>
<xml_diff>
--- a/ges_health_study_app/text_dictionary.xlsx
+++ b/ges_health_study_app/text_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sheenamartenies/Library/CloudStorage/Box-Box/Research/Projects/ges_health_study_app/ges_health_study_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9958B47-6550-404A-AAB9-42AC83FEAF0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBB09C7-0C20-2B40-B633-602D120144E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34960" yWindow="2580" windowWidth="28800" windowHeight="16320" xr2:uid="{8CCB3879-A5FF-D846-9F66-5161AE062B3F}"/>
+    <workbookView xWindow="960" yWindow="980" windowWidth="37440" windowHeight="18520" xr2:uid="{8CCB3879-A5FF-D846-9F66-5161AE062B3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -437,9 +437,6 @@
     <t>This dynamic mapping tool is a collaboration between ENVIRONS and the GES Health Study Community Council. This tool allows users to compare population characteristics and environmental exposures across neighborhoods in Denver. It was built with community data needs in mind and informed by feedback from our GES Community Council.</t>
   </si>
   <si>
-    <t>The current ENVIRONS team includes: Dr. Sheryl Magzamen, Dr. Sheena Martenies, Beth Lunsford, Anna Kenyon, Rocio Monroy-Tello, and Nona Nyart. Marshall Thomas (former ENVIRONS member) also contributed to the development of the data sets used in this tool.</t>
-  </si>
-  <si>
     <t>text_70</t>
   </si>
   <si>
@@ -694,9 +691,6 @@
     <t>Esta herramienta de mapeo dinámico es una colaboración entre ENVIRONS y el Consejo Comunitario del Estudio de Salud de GES. Esta herramienta permite a los usuarios comparar las características de la población y las exposiciones ambientales en los vecindarios de Denver. Se creó teniendo en cuenta las necesidades de datos de la comunidad y se basó en los comentarios de nuestro Consejo Comunitario de GES.</t>
   </si>
   <si>
-    <t>El equipo actual de ENVIRONS está formado por la Dra. Sheryl Magzamen, la Dra. Sheena Martenies, Beth Lunsford, Anna Kenyon, Rocio Monroy-Tello y Nona Nyart. Marshall Thomas (ex miembro de ENVIRONS) también contribuyó al desarrollo de los conjuntos de datos utilizados en esta herramienta.</t>
-  </si>
-  <si>
     <t>El estudio de salud GES también cuenta con el apoyo de un comité directivo. Entre los miembros actuales del comité directivo se encuentran: la Dra. Melinda Laituri, Aracely Navarro, Lubna Ahmed y la Dra. Rose Ediger.</t>
   </si>
   <si>
@@ -1081,9 +1075,6 @@
     <t>"When you submit a geocode request, the web server automatically collects certain technical information from your computer and about your connection. The only information that is stored is IP Address (for batch and single address submissions) and submitted address (only for single address submissions). The information is stored on a server, which is internal to the Census network.  This server is only accessible by Census Bureau staff, who are bound by the confidentiality requirements set forth in Title 13 of the United States Code and requires multiple levels of approval. This information is only used to monitor and track the performance of the Geocoder."</t>
   </si>
   <si>
-    <t>To find the neighborhood associated with an address, we use a geocoder run by the US Census Bureau. The following information from the US Census Bureau descibes how they use the address information you provide:</t>
-  </si>
-  <si>
     <t>Para encontrar el vecindario asociado con una dirección, utilizamos un geocodificador administrado por la Oficina del Censo de los EE. UU. La siguiente información de la Oficina del Censo de los EE. UU. describe cómo utilizan la información de la dirección que usted proporciona:</t>
   </si>
   <si>
@@ -1157,6 +1148,15 @@
   </si>
   <si>
     <t>&lt;a href='https://groundworkcolorado.org/'&gt;Groundwork Denver&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>To find the neighborhood associated with an address, we use a geocoder run by the US Census Bureau. The following information from the US Census Bureau describes how they use the address information you provide:</t>
+  </si>
+  <si>
+    <t>The current ENVIRONS team includes: Dr. Sheryl Magzamen, Dr. Sheena Martenies, Beth Lunsford, Anna Kenyon, Rocio Monroy-Tello, and Nona Nyhart. Marshall Thomas (former ENVIRONS member) also contributed to the development of the data sets used in this tool.</t>
+  </si>
+  <si>
+    <t>El equipo actual de ENVIRONS está formado por la Dra. Sheryl Magzamen, la Dra. Sheena Martenies, Beth Lunsford, Anna Kenyon, Rocio Monroy-Tello y Nona Nyhart. Marshall Thomas (ex miembro de ENVIRONS) también contribuyó al desarrollo de los conjuntos de datos utilizados en esta herramienta.</t>
   </si>
 </sst>
 </file>
@@ -1573,7 +1573,7 @@
   <dimension ref="A1:C128"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A62" zoomScale="92" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1600,7 +1600,7 @@
         <v>51</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>60</v>
@@ -1608,13 +1608,13 @@
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1633,10 +1633,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1677,10 +1677,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1713,7 +1713,7 @@
         <v>47</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1721,10 +1721,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="85" x14ac:dyDescent="0.2">
@@ -1732,10 +1732,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1768,7 +1768,7 @@
         <v>61</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1779,7 +1779,7 @@
         <v>62</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -1790,7 +1790,7 @@
         <v>63</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1801,7 +1801,7 @@
         <v>64</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1812,7 +1812,7 @@
         <v>65</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1823,7 +1823,7 @@
         <v>66</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1831,10 +1831,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1845,7 +1845,7 @@
         <v>67</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1856,7 +1856,7 @@
         <v>68</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1864,10 +1864,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1878,7 +1878,7 @@
         <v>69</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1889,7 +1889,7 @@
         <v>70</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1900,7 +1900,7 @@
         <v>71</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1911,7 +1911,7 @@
         <v>72</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1922,7 +1922,7 @@
         <v>73</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1933,7 +1933,7 @@
         <v>74</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="68" x14ac:dyDescent="0.2">
@@ -1941,10 +1941,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>359</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1952,10 +1952,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1966,7 +1966,7 @@
         <v>75</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -1977,7 +1977,7 @@
         <v>76</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -1985,10 +1985,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1999,7 +1999,7 @@
         <v>77</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2010,7 +2010,7 @@
         <v>78</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2021,7 +2021,7 @@
         <v>80</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2032,7 +2032,7 @@
         <v>79</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2043,7 +2043,7 @@
         <v>81</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2054,7 +2054,7 @@
         <v>82</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="68" x14ac:dyDescent="0.2">
@@ -2065,7 +2065,7 @@
         <v>113</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="85" x14ac:dyDescent="0.2">
@@ -2076,7 +2076,7 @@
         <v>114</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2087,7 +2087,7 @@
         <v>115</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -2095,10 +2095,10 @@
         <v>87</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -2109,7 +2109,7 @@
         <v>116</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="68" x14ac:dyDescent="0.2">
@@ -2120,7 +2120,7 @@
         <v>117</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2131,7 +2131,7 @@
         <v>118</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2142,7 +2142,7 @@
         <v>119</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -2153,7 +2153,7 @@
         <v>120</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -2164,7 +2164,7 @@
         <v>121</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2175,7 +2175,7 @@
         <v>122</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2186,7 +2186,7 @@
         <v>123</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="68" x14ac:dyDescent="0.2">
@@ -2197,7 +2197,7 @@
         <v>124</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="85" x14ac:dyDescent="0.2">
@@ -2205,10 +2205,10 @@
         <v>97</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -2219,7 +2219,7 @@
         <v>125</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2230,7 +2230,7 @@
         <v>126</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2241,7 +2241,7 @@
         <v>127</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="119" x14ac:dyDescent="0.2">
@@ -2252,7 +2252,7 @@
         <v>128</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="187" x14ac:dyDescent="0.2">
@@ -2263,7 +2263,7 @@
         <v>129</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="68" x14ac:dyDescent="0.2">
@@ -2274,7 +2274,7 @@
         <v>130</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2285,7 +2285,7 @@
         <v>131</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -2293,10 +2293,10 @@
         <v>105</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2304,10 +2304,10 @@
         <v>106</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2315,10 +2315,10 @@
         <v>107</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -2326,10 +2326,10 @@
         <v>108</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2337,10 +2337,10 @@
         <v>109</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="85" x14ac:dyDescent="0.2">
@@ -2351,7 +2351,7 @@
         <v>132</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="85" x14ac:dyDescent="0.2">
@@ -2359,10 +2359,10 @@
         <v>111</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -2370,626 +2370,626 @@
         <v>112</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>133</v>
+        <v>371</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>218</v>
+        <v>372</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B79" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C79" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B86" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C86" s="2" t="s">
         <v>167</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B87" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B87" s="2" t="s">
-        <v>166</v>
-      </c>
       <c r="C87" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C90" s="2" t="s">
         <v>244</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>347</v>
+        <v>370</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="136" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B125" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="C125" s="2" t="s">
         <v>346</v>
-      </c>
-      <c r="C125" s="2" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates for 2.10 Deliverable submission
</commit_message>
<xml_diff>
--- a/ges_health_study_app/text_dictionary.xlsx
+++ b/ges_health_study_app/text_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sheenamartenies/Library/CloudStorage/Box-Box/Research/Projects/ges_health_study_app/ges_health_study_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBB09C7-0C20-2B40-B633-602D120144E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{083983D5-F678-E747-A900-D12DB4F5D9AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="980" windowWidth="37440" windowHeight="18520" xr2:uid="{8CCB3879-A5FF-D846-9F66-5161AE062B3F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="37440" windowHeight="18520" xr2:uid="{8CCB3879-A5FF-D846-9F66-5161AE062B3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="386">
   <si>
     <t>text_id</t>
   </si>
@@ -573,9 +573,6 @@
   </si>
   <si>
     <t>Resumen relevante para la comunidad</t>
-  </si>
-  <si>
-    <t>Insertar aquí un resumen relevante para la comunidad</t>
   </si>
   <si>
     <t>Opciones de mapa</t>
@@ -1009,9 +1006,6 @@
     <t>Arriba se muestra un mapa interactivo que muestra los nombres de los vecindarios de Denver.</t>
   </si>
   <si>
-    <t>Insert community-relevant summary here</t>
-  </si>
-  <si>
     <t>Each unit in this map represents a census tracts. Census tracts mostly follow other natural or human-made boundaries and include about 3,000 to 6,000 people. GES is now made up of three tracts, one for Globeville, and two for the Elyria and Swansea areas. Census tracts are very useful in this study because they have the most detailed information available from the census and allow for comparison between GES and other parts of Denver.</t>
   </si>
   <si>
@@ -1081,12 +1075,6 @@
     <t>"Cuando envía una solicitud de geocodificación, el servidor web recopila automáticamente cierta información técnica de su computadora y sobre su conexión. La única información que se almacena es la dirección IP (para envíos por lotes y de una sola dirección) y la dirección enviada (solo para envíos de una sola dirección). La información se almacena en un servidor, que es interno a la red del Censo. A este servidor solo puede acceder el personal de la Oficina del Censo, que está sujeto a los requisitos de confidencialidad establecidos en el Título 13 del Código de los Estados Unidos y requiere múltiples niveles de aprobación. Esta información solo se utiliza para monitorear y hacer un seguimiento del rendimiento del geocodificador".</t>
   </si>
   <si>
-    <t>Si no desea ingresar su propia dirección, puede ingresar la dirección de una empresa local u otra ubicación en el vecindario de interés.</t>
-  </si>
-  <si>
-    <t>If you do not wish to enter your own address, you can enter the address of a local business or another location in the neighborhood of interest.</t>
-  </si>
-  <si>
     <t>Dirección:</t>
   </si>
   <si>
@@ -1157,6 +1145,57 @@
   </si>
   <si>
     <t>El equipo actual de ENVIRONS está formado por la Dra. Sheryl Magzamen, la Dra. Sheena Martenies, Beth Lunsford, Anna Kenyon, Rocio Monroy-Tello y Nona Nyhart. Marshall Thomas (ex miembro de ENVIRONS) también contribuyó al desarrollo de los conjuntos de datos utilizados en esta herramienta.</t>
+  </si>
+  <si>
+    <t>text_126</t>
+  </si>
+  <si>
+    <t>text_127</t>
+  </si>
+  <si>
+    <t>text_128</t>
+  </si>
+  <si>
+    <t>text_129</t>
+  </si>
+  <si>
+    <t>text_130</t>
+  </si>
+  <si>
+    <t>If you live in a community outside of the GES neighborhoods, our summary and excitement for this particular tool might be hard to understand. We can imagine that in other neighborhoods, a new tool showing data about levels of pollution or short life expectancies, that indicate visually the “numbers” of the problems, may be unnecessary. Stay tuned, however, because other communities have a role to play in this new development. In the GES neighborhoods, we are continuously looking for new ways to communicate our lived experiences more clearly with those who are willing to learn and listen. This new map may be the next step towards that.  </t>
+  </si>
+  <si>
+    <t>This tool helps present data clearly and visually, making it easier to highlight problems. For example, this tool can show the density of marijuana dispensaries compared to food stores and the health impacts of pollution and proximity to I-70. It provides residents with concrete data to advocate for change, communicate concerns to representatives, and take collective action without relying solely on individual experiences. What's particularly interesting about this tool, is that we can compare our data directly to the data of other communities. What are the asthma or cancer rates in your community compared to ours? Take a look yourself. This tool allows you to select from a wide range of data to compare so you can look into what matters most to you and your family.  </t>
+  </si>
+  <si>
+    <t>As a community, we’ve spent countless hours without feeling heard when we describe what it's like to live in communities adjacent to highways and heavy industry. Clear data is essential to having our lived experiences believed by advocates, legislators, and policymakers who, up until now, have not been held accountable for their promises. As a working-class community, having a tool that shows the stark differences between our struggles and those of other Denver communities may help legislators and allies understand that the GES neighborhoods are not being heard.  </t>
+  </si>
+  <si>
+    <t>Finally, this tool is validating. As a working-class community, it is energy-consuming and demoralizing to go through pages and pages of hard-to-understand numbers and data and then extremely time-consuming to call city hotlines to report every problem- we’d be on the phone as a full-time job.  When we have called, we feel that corrections are minimal and any response at all is days delayed. This tool is quick, customizable, and easier to understand than elaborate spreadsheets. We can describe the odors we smell, or tell stories of how many friends we have lost due to our proximity to deep polluters, but it isn't until we can see our stories that we are able to feel that our struggles are real and more easily communicated.  </t>
+  </si>
+  <si>
+    <t>- Your GES Health Study Community Council</t>
+  </si>
+  <si>
+    <t>The use of the "Find a Neighborhood" tool is optional. If you do not wish to enter your own address, you can enter the address of a local business or another location in the neighborhood of interest.</t>
+  </si>
+  <si>
+    <t>El uso de la herramienta "Buscar un barrio" es opcional. Si no desea ingresar su propia dirección, puede ingresar la dirección de un negocio local u otra ubicación en el barrio de interés.</t>
+  </si>
+  <si>
+    <t>Si vives en una comunidad fuera de los vecindarios de GES, puede que no entiendas nuestro resumen y entusiasmo por esta herramienta en particular. Podemos imaginar que en otros vecindarios, una nueva herramienta que muestre datos sobre los niveles de contaminación o las cortas expectativas de vida, que indiquen visualmente los “números” de los problemas, puede resultar innecesaria. Sin embargo, permanece atento, porque otras comunidades tienen un papel que desempeñar en este nuevo desarrollo. En los vecindarios de GES, buscamos continuamente nuevas formas de comunicar nuestras experiencias vividas de forma más clara a quienes están dispuestos a aprender y escuchar. Este nuevo mapa puede ser el siguiente paso en esa dirección.</t>
+  </si>
+  <si>
+    <t>Esta herramienta ayuda a presentar los datos de forma clara y visual, lo que facilita la identificación de los problemas. Por ejemplo, esta herramienta puede mostrar la densidad de dispensarios de marihuana en comparación con las tiendas de alimentos y los impactos en la salud de la contaminación y la proximidad a la I-70. Proporciona a los residentes datos concretos para abogar por el cambio, comunicar inquietudes a los representantes y tomar medidas colectivas sin depender únicamente de las experiencias individuales. Lo que resulta particularmente interesante de esta herramienta es que podemos comparar nuestros datos directamente con los datos de otras comunidades. ¿Cuáles son las tasas de asma o cáncer en su comunidad en comparación con las nuestras? Eche un vistazo usted mismo. Esta herramienta le permite seleccionar entre una amplia gama de datos para comparar, de modo que pueda analizar lo que más le importa a usted y a su familia.</t>
+  </si>
+  <si>
+    <t>Como comunidad, hemos pasado incontables horas sin sentirnos escuchados cuando describimos cómo es vivir en comunidades adyacentes a autopistas e industria pesada. Es esencial contar con datos claros para que los defensores, legisladores y legisladores que, hasta ahora, no han tenido que rendir cuentas de sus promesas, crean en nuestras experiencias vividas. Como comunidad de clase trabajadora, contar con una herramienta que muestre las marcadas diferencias entre nuestras luchas y las de otras comunidades de Denver puede ayudar a los legisladores y aliados a comprender que los vecindarios de GES no están siendo escuchados.</t>
+  </si>
+  <si>
+    <t>Finalmente, esta herramienta es validadora. Como comunidad de clase trabajadora, consume energía y es desmoralizante revisar páginas y páginas de números y datos difíciles de entender y luego consume muchísimo tiempo llamar a las líneas directas de la ciudad para informar cada problema; estaríamos en el teléfono como un trabajo de tiempo completo. Cuando hemos llamado, sentimos que las correcciones son mínimas y cualquier respuesta se demora días. Esta herramienta es rápida, personalizable y más fácil de entender que las elaboradas hojas de cálculo. Podemos describir los olores que olemos o contar historias de cuántos amigos hemos perdido debido a nuestra proximidad a contaminadores profundos, pero no es hasta que podemos ver nuestras historias que podemos sentir que nuestras luchas son reales y más fáciles de comunicar.</t>
+  </si>
+  <si>
+    <t>- Su Consejo Comunitario de Estudios de Salud GES</t>
   </si>
 </sst>
 </file>
@@ -1195,18 +1234,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1227,13 +1260,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1570,10 +1603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{548E5ED1-4340-C04D-8029-23B2D57DC5C7}">
-  <dimension ref="A1:C128"/>
+  <dimension ref="A1:C133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="92" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="92" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C131" sqref="C131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1608,13 +1641,13 @@
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>232</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1677,10 +1710,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>297</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1713,7 +1746,7 @@
         <v>47</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1721,10 +1754,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="85" x14ac:dyDescent="0.2">
@@ -1732,10 +1765,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1768,7 +1801,7 @@
         <v>61</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1790,7 +1823,7 @@
         <v>63</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1812,7 +1845,7 @@
         <v>65</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1834,7 +1867,7 @@
         <v>176</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1844,7 +1877,7 @@
       <c r="B24" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="4" t="s">
         <v>177</v>
       </c>
     </row>
@@ -1859,15 +1892,9 @@
         <v>178</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1878,7 +1905,7 @@
         <v>69</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1889,7 +1916,7 @@
         <v>70</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1900,7 +1927,7 @@
         <v>71</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1911,7 +1938,7 @@
         <v>72</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1922,7 +1949,7 @@
         <v>73</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1933,7 +1960,7 @@
         <v>74</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="68" x14ac:dyDescent="0.2">
@@ -1941,10 +1968,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1952,10 +1979,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1966,7 +1993,7 @@
         <v>75</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -1977,7 +2004,7 @@
         <v>76</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -1985,10 +2012,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>227</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1999,7 +2026,7 @@
         <v>77</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2010,7 +2037,7 @@
         <v>78</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2021,7 +2048,7 @@
         <v>80</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2032,7 +2059,7 @@
         <v>79</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2043,7 +2070,7 @@
         <v>81</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2054,7 +2081,7 @@
         <v>82</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="68" x14ac:dyDescent="0.2">
@@ -2065,7 +2092,7 @@
         <v>113</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="85" x14ac:dyDescent="0.2">
@@ -2076,7 +2103,7 @@
         <v>114</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2087,7 +2114,7 @@
         <v>115</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -2098,7 +2125,7 @@
         <v>155</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -2109,7 +2136,7 @@
         <v>116</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="68" x14ac:dyDescent="0.2">
@@ -2120,7 +2147,7 @@
         <v>117</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2131,7 +2158,7 @@
         <v>118</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2142,7 +2169,7 @@
         <v>119</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -2153,7 +2180,7 @@
         <v>120</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -2164,7 +2191,7 @@
         <v>121</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2175,7 +2202,7 @@
         <v>122</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2186,7 +2213,7 @@
         <v>123</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="68" x14ac:dyDescent="0.2">
@@ -2197,7 +2224,7 @@
         <v>124</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="85" x14ac:dyDescent="0.2">
@@ -2205,10 +2232,10 @@
         <v>97</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -2219,7 +2246,7 @@
         <v>125</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2230,7 +2257,7 @@
         <v>126</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2241,7 +2268,7 @@
         <v>127</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="119" x14ac:dyDescent="0.2">
@@ -2252,7 +2279,7 @@
         <v>128</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="187" x14ac:dyDescent="0.2">
@@ -2263,7 +2290,7 @@
         <v>129</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="68" x14ac:dyDescent="0.2">
@@ -2274,7 +2301,7 @@
         <v>130</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2285,7 +2312,7 @@
         <v>131</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -2293,10 +2320,10 @@
         <v>105</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2304,10 +2331,10 @@
         <v>106</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2315,10 +2342,10 @@
         <v>107</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -2326,10 +2353,10 @@
         <v>108</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2337,10 +2364,10 @@
         <v>109</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="85" x14ac:dyDescent="0.2">
@@ -2351,7 +2378,7 @@
         <v>132</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="85" x14ac:dyDescent="0.2">
@@ -2359,10 +2386,10 @@
         <v>111</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -2370,10 +2397,10 @@
         <v>112</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -2384,7 +2411,7 @@
         <v>145</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -2395,7 +2422,7 @@
         <v>146</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -2403,10 +2430,10 @@
         <v>135</v>
       </c>
       <c r="B75" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C75" s="2" t="s">
         <v>219</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -2417,7 +2444,7 @@
         <v>147</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2428,7 +2455,7 @@
         <v>148</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -2436,10 +2463,10 @@
         <v>138</v>
       </c>
       <c r="B78" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C78" s="2" t="s">
         <v>223</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2543,453 +2570,508 @@
     </row>
     <row r="88" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B88" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="B88" s="2" t="s">
-        <v>226</v>
-      </c>
       <c r="C88" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="C89" s="4" t="s">
-        <v>352</v>
+        <v>347</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B90" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="C90" s="2" t="s">
         <v>243</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B91" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="B91" s="2" t="s">
-        <v>246</v>
-      </c>
       <c r="C91" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B98" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C98" s="2" t="s">
         <v>266</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B109" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="C109" s="2" t="s">
         <v>300</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B110" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C110" s="1" t="s">
         <v>309</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B111" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C111" s="2" t="s">
         <v>321</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="136" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B125" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C125" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="C125" s="2" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="126" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>348</v>
+        <v>379</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>347</v>
+        <v>380</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B128" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="119" x14ac:dyDescent="0.2">
+      <c r="A129" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="C128" s="2" t="s">
-        <v>369</v>
+      <c r="B129" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" ht="153" x14ac:dyDescent="0.2">
+      <c r="A130" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" ht="119" x14ac:dyDescent="0.2">
+      <c r="A131" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="136" x14ac:dyDescent="0.2">
+      <c r="A132" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A133" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B133" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="C133" s="5" t="s">
+        <v>385</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correcting the name of the study: GES Community Health Study
</commit_message>
<xml_diff>
--- a/ges_health_study_app/text_dictionary.xlsx
+++ b/ges_health_study_app/text_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sheenamartenies/Library/CloudStorage/Box-Box/Research/Projects/ges_health_study_app/ges_health_study_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{083983D5-F678-E747-A900-D12DB4F5D9AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F4E8BA-8BF3-A446-B048-C53C68829882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="37440" windowHeight="18520" xr2:uid="{8CCB3879-A5FF-D846-9F66-5161AE062B3F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{8CCB3879-A5FF-D846-9F66-5161AE062B3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -164,18 +164,9 @@
     <t>text_39</t>
   </si>
   <si>
-    <t>GES Health Study Interactive Maps</t>
-  </si>
-  <si>
-    <t>Welcome to the GES Health Study Interactive Maps app! We are excited to share this important tool with you. The Interactive Maps app was developed to help community members learn more about the environmental conditions that currently and historically exist in the Globeville, Elyria, and Swansea neighborhoods of Denver.</t>
-  </si>
-  <si>
     <t>Globeville, Elyria, and Swansea (GES) are neighborhoods in the North Denver area bordering Commerce City. Officially designated as Globeville and Elyria-Swansea by the city of Denver, these communities are some of the oldest in Denver. Today, the neighborhoods are home to a vibrant Hispanic culture, which intertwines with the heritage of the European immigrants who originally lived in the area to create a community unlike anywhere else in Denver. The more than 11,000 residents of GES contend with poor environmental quality and encroachment by a growing city while fighting to maintain the community and culture they call home.</t>
   </si>
   <si>
-    <t>We invite you to continue reading to learn more about the GES Health Study Interactive Maps app.</t>
-  </si>
-  <si>
     <t>From the Community Council</t>
   </si>
   <si>
@@ -188,9 +179,6 @@
     <t>Community Maps</t>
   </si>
   <si>
-    <t>Mapas interactivos del estudio de salud de GES</t>
-  </si>
-  <si>
     <t>text_switch</t>
   </si>
   <si>
@@ -200,9 +188,6 @@
     <t>Welcome!</t>
   </si>
   <si>
-    <t>¡Bienvenido a la aplicación de mapas interactivos del estudio de salud de GES! Nos complace compartir esta importante herramienta con usted. La aplicación de mapas interactivos se desarrolló para ayudar a los miembros de la comunidad a aprender más sobre las condiciones ambientales que existen actualmente e históricamente en los vecindarios de Globeville, Elyria y Swansea de Denver.</t>
-  </si>
-  <si>
     <t>Globeville, Elyria y Swansea (GES) son vecindarios en el área del norte de Denver que limitan con Commerce City. Designadas oficialmente como Globeville y Elyria-Swansea por la ciudad de Denver, estas comunidades son algunas de las más antiguas de Denver. Hoy, los vecindarios albergan una vibrante cultura hispana, que se entrelaza con la herencia de los inmigrantes europeos que originalmente vivían en el área para crear una comunidad diferente a cualquier otro lugar de Denver. Los más de 11.000 residentes de GES se enfrentan a una mala calidad ambiental y a la invasión de una ciudad en crecimiento mientras luchan por mantener la comunidad y la cultura que consideran su hogar.</t>
   </si>
   <si>
@@ -218,9 +203,6 @@
     <t>Mapas de la comunidad</t>
   </si>
   <si>
-    <t>Read this site in English: &lt;a href='https://smartenies.shinyapps.io/ges_health_study_app_english'&gt; GES Health Study Interactive Maps&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>On the &lt;b&gt;Community Maps&lt;/b&gt; tab, you'll be able to explore the maps highlighting locations in Globeville, Elyria, and Swansea identified by GES community council members and neighborhood residents as locations of community pride and community concern. Data presented in these maps were collected during a series of activities and meetings conducted in 2022 and 2023.</t>
   </si>
   <si>
@@ -380,15 +362,9 @@
     <t>In 2022 and 2023, residents of Globeville, Elyria, and Swansea (GES) shared locations that help describe what it is like to live in GES. The map below represents the points residents marked in response to questions about areas of community pride, gathering, and concern, as well as where they go to buy groceries and access health care.</t>
   </si>
   <si>
-    <t>More information about this map and our findings can be found on the &lt;a href='https://www.geshealthstudy.org/maps/community-mapping-locations'&gt; GES Health Study website&lt;/a&gt;.</t>
-  </si>
-  <si>
     <t>Community Mapping Results</t>
   </si>
   <si>
-    <t>In addition to our community mapping exercise, the GES health study has generated a number of maps documenting environmental and health conditions in the GES neighborhoods. We have included these maps here for you to explore.</t>
-  </si>
-  <si>
     <t>More information about the about health and the environment in the GES neighborhoods can be found in our 2023 Health Impact Assessment: &lt;a href='https://www.geshealthstudy.org/products#h.qz2fxzwvkzcz'&gt; The ABC's of GES: The State of Health and Environment&lt;/a&gt;, which is available in both English and Spanish.</t>
   </si>
   <si>
@@ -546,9 +522,6 @@
   </si>
   <si>
     <t>Fuente de datos:</t>
-  </si>
-  <si>
-    <t>Lea este sitio en español: &lt;a href='https://smartenies.shinyapps.io/ges_health_study_app_espanol'&gt; Mapas interactivos del estudio de salud de GES&lt;/a&gt;</t>
   </si>
   <si>
     <t>Start Here/Empieza aquí</t>
@@ -634,9 +607,6 @@
     <t>Fuente: Datos primarios solicitados al Consejo Comunitario y a miembros de la comunidad de GES. Actualizado el 15/02/23.</t>
   </si>
   <si>
-    <t>Además de nuestro ejercicio de mapeo comunitario, el estudio de salud de GES ha generado una serie de mapas que documentan las condiciones ambientales y de salud en los vecindarios de GES. Hemos incluido estos mapas aquí para que los explore.</t>
-  </si>
-  <si>
     <t>Puede encontrar más información sobre la salud y el medio ambiente en los vecindarios de GES en nuestra Evaluación de Impacto en la Salud de 2023: &lt;a href='https://www.geshealthstudy.org/products#h.qz2fxzwvkzcz'&gt;El ABC de GES: El estado de la salud y el medio ambiente&lt;/a&gt;, que está disponible en inglés y español.</t>
   </si>
   <si>
@@ -685,15 +655,9 @@
     <t>Recursos para aprender más</t>
   </si>
   <si>
-    <t>Esta herramienta de mapeo dinámico es una colaboración entre ENVIRONS y el Consejo Comunitario del Estudio de Salud de GES. Esta herramienta permite a los usuarios comparar las características de la población y las exposiciones ambientales en los vecindarios de Denver. Se creó teniendo en cuenta las necesidades de datos de la comunidad y se basó en los comentarios de nuestro Consejo Comunitario de GES.</t>
-  </si>
-  <si>
     <t>El estudio de salud GES también cuenta con el apoyo de un comité directivo. Entre los miembros actuales del comité directivo se encuentran: la Dra. Melinda Laituri, Aracely Navarro, Lubna Ahmed y la Dra. Rose Ediger.</t>
   </si>
   <si>
-    <t>Puede encontrar más información sobre el Consejo Comunitario de GES, el equipo ENVRONS y el Comité Directivo del Estudio de Salud de GES en nuestro sitio web: &lt;a href='https://www.geshealthstudy.org/about/who-we-are'&gt;Estudio de Salud Comunitaria de GES&lt;/a&gt;.</t>
-  </si>
-  <si>
     <t>Map showing locations identified by GES community members as both positive and negative influences on their health and wellbeing.</t>
   </si>
   <si>
@@ -1196,6 +1160,42 @@
   </si>
   <si>
     <t>- Su Consejo Comunitario de Estudios de Salud GES</t>
+  </si>
+  <si>
+    <t>Read this site in English: &lt;a href='https://smartenies.shinyapps.io/ges_health_study_app_english'&gt; GES Community Health Study Interactive Maps&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>GES Community Health Study Interactive Maps</t>
+  </si>
+  <si>
+    <t>Welcome to the GES Community Health Study Interactive Maps app! We are excited to share this important tool with you. The Interactive Maps app was developed to help community members learn more about the environmental conditions that currently and historically exist in the Globeville, Elyria, and Swansea neighborhoods of Denver.</t>
+  </si>
+  <si>
+    <t>We invite you to continue reading to learn more about the GES Community Health Study Interactive Maps app.</t>
+  </si>
+  <si>
+    <t>More information about this map and our findings can be found on the &lt;a href='https://www.geshealthstudy.org/maps/community-mapping-locations'&gt; GES Community Health Study website&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>In addition to our community mapping exercise, the GES Community Health Study has generated a number of maps documenting environmental and health conditions in the GES neighborhoods. We have included these maps here for you to explore.</t>
+  </si>
+  <si>
+    <t>Lea este sitio en español: &lt;a href='https://smartenies.shinyapps.io/ges_health_study_app_espanol'&gt; Mapas interactivos del Estudio de salud comunitaria del GES&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Mapas interactivos del Estudio de salud comunitaria del GES</t>
+  </si>
+  <si>
+    <t>¡Bienvenido a la aplicación de mapas interactivos del Estudio de salud comunitaria del GES! Nos complace compartir esta importante herramienta con usted. La aplicación de mapas interactivos se desarrolló para ayudar a los miembros de la comunidad a aprender más sobre las condiciones ambientales que existen actualmente e históricamente en los vecindarios de Globeville, Elyria y Swansea de Denver.</t>
+  </si>
+  <si>
+    <t>Además de nuestro ejercicio de mapeo comunitario, el Estudio de salud comunitaria del GES ha generado una serie de mapas que documentan las condiciones ambientales y de salud en los vecindarios de GES. Hemos incluido estos mapas aquí para que los explore.</t>
+  </si>
+  <si>
+    <t>Esta herramienta de mapeo dinámico es una colaboración entre ENVIRONS y el Consejo Comunitario del Estudio de salud comunitaria del GES. Esta herramienta permite a los usuarios comparar las características de la población y las exposiciones ambientales en los vecindarios de Denver. Se creó teniendo en cuenta las necesidades de datos de la comunidad y se basó en los comentarios de nuestro Consejo Comunitario de GES.</t>
+  </si>
+  <si>
+    <t>Puede encontrar más información sobre el Consejo Comunitario de GES, el equipo ENVRONS y el Comité Directivo del Estudio de salud comunitaria del GES en nuestro sitio web: &lt;a href='https://www.geshealthstudy.org/about/who-we-are'&gt;Estudio de Salud Comunitaria de GES&lt;/a&gt;.</t>
   </si>
 </sst>
 </file>
@@ -1605,8 +1605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{548E5ED1-4340-C04D-8029-23B2D57DC5C7}">
   <dimension ref="A1:C133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="92" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C131" sqref="C131"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="92" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1630,24 +1630,24 @@
     </row>
     <row r="2" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>170</v>
+        <v>380</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>60</v>
+        <v>374</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1655,10 +1655,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>42</v>
+        <v>375</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>50</v>
+        <v>381</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1666,10 +1666,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1677,10 +1677,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="68" x14ac:dyDescent="0.2">
@@ -1688,10 +1688,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>43</v>
+        <v>376</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>54</v>
+        <v>382</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="119" x14ac:dyDescent="0.2">
@@ -1699,10 +1699,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="102" x14ac:dyDescent="0.2">
@@ -1710,10 +1710,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1721,10 +1721,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>45</v>
+        <v>377</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1732,10 +1732,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1743,10 +1743,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1754,10 +1754,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="85" x14ac:dyDescent="0.2">
@@ -1765,10 +1765,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1776,10 +1776,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1787,10 +1787,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="85" x14ac:dyDescent="0.2">
@@ -1798,10 +1798,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1809,10 +1809,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -1820,10 +1820,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1831,10 +1831,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1842,10 +1842,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1853,10 +1853,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1864,10 +1864,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1875,10 +1875,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1886,10 +1886,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -1902,10 +1902,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1913,10 +1913,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1924,10 +1924,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1935,10 +1935,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1946,10 +1946,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1957,10 +1957,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="68" x14ac:dyDescent="0.2">
@@ -1968,10 +1968,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>352</v>
+        <v>340</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>355</v>
+        <v>343</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1979,10 +1979,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1990,10 +1990,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -2001,10 +2001,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -2012,10 +2012,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2023,10 +2023,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2034,10 +2034,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2045,10 +2045,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2056,10 +2056,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2067,1011 +2067,1011 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>114</v>
+        <v>378</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>116</v>
+        <v>379</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>198</v>
+        <v>383</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>322</v>
+        <v>310</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="119" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="187" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>359</v>
+        <v>347</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>361</v>
+        <v>349</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>361</v>
+        <v>349</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>362</v>
+        <v>350</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>362</v>
+        <v>350</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>215</v>
+        <v>384</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>350</v>
+        <v>338</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>367</v>
+        <v>355</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>368</v>
+        <v>356</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>217</v>
+        <v>385</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>354</v>
+        <v>342</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="C95" s="2" t="s">
         <v>250</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B96" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="B96" s="2" t="s">
-        <v>263</v>
-      </c>
       <c r="C96" s="2" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B97" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="B97" s="2" t="s">
-        <v>264</v>
-      </c>
       <c r="C97" s="2" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B98" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="B98" s="2" t="s">
-        <v>265</v>
-      </c>
       <c r="C98" s="2" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>292</v>
+        <v>280</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>280</v>
+        <v>268</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>281</v>
+        <v>269</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>309</v>
+        <v>297</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>320</v>
+        <v>308</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>321</v>
+        <v>309</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>310</v>
+        <v>298</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>315</v>
+        <v>303</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>316</v>
+        <v>304</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>312</v>
+        <v>300</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>317</v>
+        <v>305</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>304</v>
+        <v>292</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>313</v>
+        <v>301</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>318</v>
+        <v>306</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>314</v>
+        <v>302</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>319</v>
+        <v>307</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>306</v>
+        <v>294</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>326</v>
+        <v>314</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>327</v>
+        <v>315</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>332</v>
+        <v>320</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>335</v>
+        <v>323</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>328</v>
+        <v>316</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>333</v>
+        <v>321</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>336</v>
+        <v>324</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>329</v>
+        <v>317</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>330</v>
+        <v>318</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C123" s="2" t="s">
         <v>337</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="C123" s="2" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>366</v>
+        <v>354</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>343</v>
+        <v>331</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="136" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>339</v>
+        <v>327</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>379</v>
+        <v>367</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>380</v>
+        <v>368</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>364</v>
+        <v>352</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>364</v>
+        <v>352</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="136" x14ac:dyDescent="0.2">
+      <c r="A129" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="B128" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="C128" s="2" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" ht="119" x14ac:dyDescent="0.2">
-      <c r="A129" s="1" t="s">
+      <c r="B129" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="C129" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="B129" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="C129" s="2" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" ht="153" x14ac:dyDescent="0.2">
+    </row>
+    <row r="130" spans="1:3" ht="170" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="C130" s="2" t="s">
         <v>370</v>
-      </c>
-      <c r="B130" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="C130" s="2" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="119" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="C131" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="B131" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="C131" s="2" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" ht="136" x14ac:dyDescent="0.2">
+    </row>
+    <row r="132" spans="1:3" ht="153" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="C132" s="2" t="s">
         <v>372</v>
-      </c>
-      <c r="B132" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="C132" s="2" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B133" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="C133" s="5" t="s">
         <v>373</v>
-      </c>
-      <c r="B133" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="C133" s="5" t="s">
-        <v>385</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates in response to steering committee comments
</commit_message>
<xml_diff>
--- a/ges_health_study_app/text_dictionary.xlsx
+++ b/ges_health_study_app/text_dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sheenamartenies/Library/CloudStorage/Box-Box/Research/Projects/ges_health_study_app/ges_health_study_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F4E8BA-8BF3-A446-B048-C53C68829882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271962A7-64A8-B944-AA4D-4D98F3015327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{8CCB3879-A5FF-D846-9F66-5161AE062B3F}"/>
+    <workbookView xWindow="-36380" yWindow="1040" windowWidth="33840" windowHeight="19280" xr2:uid="{8CCB3879-A5FF-D846-9F66-5161AE062B3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="428">
   <si>
     <t>text_id</t>
   </si>
@@ -1196,6 +1196,132 @@
   </si>
   <si>
     <t>Puede encontrar más información sobre el Consejo Comunitario de GES, el equipo ENVRONS y el Comité Directivo del Estudio de salud comunitaria del GES en nuestro sitio web: &lt;a href='https://www.geshealthstudy.org/about/who-we-are'&gt;Estudio de Salud Comunitaria de GES&lt;/a&gt;.</t>
+  </si>
+  <si>
+    <t>text_131</t>
+  </si>
+  <si>
+    <t>text_132</t>
+  </si>
+  <si>
+    <t>text_133</t>
+  </si>
+  <si>
+    <t>text_134</t>
+  </si>
+  <si>
+    <t>text_135</t>
+  </si>
+  <si>
+    <t>text_136</t>
+  </si>
+  <si>
+    <t>text_137</t>
+  </si>
+  <si>
+    <t>text_138</t>
+  </si>
+  <si>
+    <t>text_139</t>
+  </si>
+  <si>
+    <t>text_140</t>
+  </si>
+  <si>
+    <t>text_141</t>
+  </si>
+  <si>
+    <t>text_142</t>
+  </si>
+  <si>
+    <t>text_143</t>
+  </si>
+  <si>
+    <t>text_144</t>
+  </si>
+  <si>
+    <t>text_145</t>
+  </si>
+  <si>
+    <t>text_146</t>
+  </si>
+  <si>
+    <t>text_147</t>
+  </si>
+  <si>
+    <t>text_148</t>
+  </si>
+  <si>
+    <t>text_149</t>
+  </si>
+  <si>
+    <t>text_150</t>
+  </si>
+  <si>
+    <t>text_151</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;Variable: &lt;/strong&gt; A data item that can change or take on more than one value </t>
+  </si>
+  <si>
+    <t>&lt;strong&gt;Distribution: &lt;/strong&gt; The range of values a data item can take on</t>
+  </si>
+  <si>
+    <t>&lt;strong&gt;Geocode: &lt;/strong&gt; A technique that identifies the location of an address on a map using geographical coordinates (longitude and latitude) so that it can be shown on a map.</t>
+  </si>
+  <si>
+    <t>&lt;strong&gt;SNAP: &lt;/strong&gt; Supplemental Nutrition Assistance Program (also known as food stamps)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;ENVIRONS: &lt;/strong&gt; Estudio de Nuestros Vecinos para Investigar los RiesgOs y Nuestra Salud (ENVIRONS) research team is based out of Colorado State University in Fort Collins, CO and is responsible for conducting the GES Community Health Study. </t>
+  </si>
+  <si>
+    <t>&lt;strong&gt;PM2.5: &lt;/strong&gt; Particulate matter that is smaller than 2.5 micrometers in diamater; PM contains microscopic solids or liquid droplets that can be inhaled and cause serious health problems. Some particles less than 2.5 micrometers in diameter can get deep into your lungs and some may even get into your bloodstream.</t>
+  </si>
+  <si>
+    <t>&lt;strong&gt;PM10: &lt;/strong&gt; Particulate matter that is smaller than 10 micrometers in diamater; PM contains microscopic solids or liquid droplets that can be inhaled and cause serious health problems.</t>
+  </si>
+  <si>
+    <t>&lt;strong&gt;NO2: &lt;/strong&gt; Nitrogen dioxide; a type of air pollutant that comes from combustion sources like car engines and industrial facilities.</t>
+  </si>
+  <si>
+    <t>&lt;strong&gt;O3: &lt;/strong&gt; Ozone; a type of air pollutant that forms when nitrogen dioxide and volatile organic compounds interact with each other in the presence of sunlight</t>
+  </si>
+  <si>
+    <t>&lt;strong&gt;SO2: &lt;/strong&gt; Sulfur dioxide; a type of air pollutant that comes primarily from coal and diesel fuel combustion</t>
+  </si>
+  <si>
+    <t>&lt;strong&gt;CO: &lt;/strong&gt; Carbon monoxide; a type of air pollutant that comes from combustion sources like car engines and industrial facilities.</t>
+  </si>
+  <si>
+    <t>&lt;strong&gt;Neighborhoods: &lt;/strong&gt; The City and County of Denver recognizes 78 official neighborhoods, including Denver International Airport (DIA). These are often made up of a collection of census tracts. For example, GES includes three census tracts.</t>
+  </si>
+  <si>
+    <t>&lt;strong&gt;Histogram: &lt;/strong&gt; A type of chart that shows the distribution of a variable. The histograms in the app show the range of values for a variable on the bottom. These ranges are divided into 30 bins. The height of each bar represents the number of neighborhoods in the bin.</t>
+  </si>
+  <si>
+    <t>Key Definitions and Acronyms</t>
+  </si>
+  <si>
+    <t>On the &lt;b&gt;Key Definitions&lt;/b&gt; tab, you'll find explanations for many of the terms used in this interactive map application.</t>
+  </si>
+  <si>
+    <t>Definitions for terms and acronyms found in the Interactive Maps App:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;GES: &lt;/strong&gt; Globeville, Elyria, and Swansea </t>
+  </si>
+  <si>
+    <t>This map include several layers that represent different variables. Click on the layer icon in the top right corner of the map to select a variable of interest.</t>
+  </si>
+  <si>
+    <t>&lt;strong&gt;CHD: &lt;/strong&gt; Coronary Heart Disease</t>
+  </si>
+  <si>
+    <t>&lt;strong&gt;COPD: &lt;/strong&gt; Chronic Obstructive Pulmonary Disease</t>
+  </si>
+  <si>
+    <t>&lt;strong&gt;Chart: &lt;/strong&gt; A visual representation of data</t>
   </si>
 </sst>
 </file>
@@ -1603,10 +1729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{548E5ED1-4340-C04D-8029-23B2D57DC5C7}">
-  <dimension ref="A1:C133"/>
+  <dimension ref="A1:C154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="92" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A132" zoomScale="92" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B137" sqref="B137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3074,7 +3200,178 @@
         <v>373</v>
       </c>
     </row>
+    <row r="134" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A134" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A135" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A136" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A137" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A138" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A139" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A140" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A141" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A142" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A143" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A144" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A145" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A146" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A147" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A148" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A149" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A150" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A151" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A152" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A153" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A154" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>424</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B137:B153">
+    <sortCondition ref="B137:B153"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updating readme and embedded links to reflect new website URL
</commit_message>
<xml_diff>
--- a/ges_health_study_app/text_dictionary.xlsx
+++ b/ges_health_study_app/text_dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uillinoisedu.sharepoint.com/sites/MarteniesLab2/Shared Documents/HELE Lab/projects/ges_health_study/data_analysis/ges_health_study_app/ges_health_study_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{271962A7-64A8-B944-AA4D-4D98F3015327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{19C3E113-E7DC-EC40-9760-0579A99356C7}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{271962A7-64A8-B944-AA4D-4D98F3015327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3BD903DD-CF80-AA41-99D0-A179FF7E0E59}"/>
   <bookViews>
-    <workbookView xWindow="-36380" yWindow="1040" windowWidth="33840" windowHeight="19280" xr2:uid="{8CCB3879-A5FF-D846-9F66-5161AE062B3F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{8CCB3879-A5FF-D846-9F66-5161AE062B3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="453">
   <si>
     <t>text_id</t>
   </si>
@@ -911,9 +911,6 @@
     <t>In addition to our community mapping exercise, the GES Community Health Study has generated a number of maps documenting environmental and health conditions in the GES neighborhoods. We have included these maps here for you to explore.</t>
   </si>
   <si>
-    <t>Lea este sitio en español: &lt;a href='https://smartenies.shinyapps.io/ges_health_study_app_espanol'&gt; Mapas interactivos del Estudio de salud comunitaria del GES&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>text_131</t>
   </si>
   <si>
@@ -1382,16 +1379,22 @@
     <t>text_152</t>
   </si>
   <si>
-    <t>&lt;strong&gt;Recommended Citation: &lt;/strong&gt; Estudio de Nuestros Vecinos para Investigar los Riesgos y Nuestra Salud (ENVIRONS). April 2025. GES Community Health Study Interactive Maps. Fort Collins, CO.</t>
-  </si>
-  <si>
-    <t>&lt;strong&gt;Cita recomendada: &lt;/strong&gt; Estudio de Nuestros Vecinos para Investigar los Riesgos y Nuestra Salud (ENVIRONS). Abril de 2025. Mapas Interactivos del Estudio de Salud Comunitaria GES. Fort Collins, CO.</t>
-  </si>
-  <si>
     <t>&lt;b&gt;How to use this app:&lt;/b&gt; This app includes tools to help users understand better the distribution of environmental exposures and health outcomes across Denver. The purpose of this app is to document trends in the social and environmental factors that impact health in Denver neighborhoods so that community residents can learn more about the conditions that exist where they live.  The data available in this app should not be used to make determinations about specific causes of health or disease for any resident living in Denver.</t>
   </si>
   <si>
     <t>&lt;b&gt;Cómo utilizar esta aplicación:&lt;/b&gt; Esta aplicación incluye herramientas para ayudar a los usuarios a comprender mejor la distribución de exposiciones ambientales y resultados de salud en Denver. El propósito de esta aplicación es documentar las tendencias en los factores sociales y ambientales que impactan la salud en los vecindarios de Denver, para que los residentes de la comunidad puedan aprender más sobre las condiciones que existen donde viven. Los datos disponibles en esta aplicación no deben utilizarse para hacer determinaciones sobre las causas específicas de la salud o enfermedades de cualquier residente que viva en Denver.</t>
+  </si>
+  <si>
+    <t>Lea este sitio en español: &lt;a href='https://geshealthstudy.shinyapps.io/ges_health_study_app_espanol'&gt; Mapas interactivos del Estudio de salud comunitaria del GES&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Lea este sitio en inglés: &lt;a href='https://geshealthstudy.shinyapps.io/ges_health_study_app_english'&gt; Mapas interactivos del Estudio de salud comunitaria del GES&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;strong&gt;Recommended Citation: &lt;/strong&gt; Estudio de Nuestros Vecinos para Investigar los Riesgos y Nuestra Salud (ENVIRONS). February 2025. GES Community Health Study Interactive Maps. Fort Collins, CO.</t>
+  </si>
+  <si>
+    <t>&lt;strong&gt;Cita recomendada: &lt;/strong&gt; Estudio de Nuestros Vecinos para Investigar los Riesgos y Nuestra Salud (ENVIRONS). Febrero de 2025. Mapas Interactivos del Estudio de Salud Comunitaria GES. Fort Collins, CO.</t>
   </si>
 </sst>
 </file>
@@ -1801,8 +1804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{548E5ED1-4340-C04D-8029-23B2D57DC5C7}">
   <dimension ref="A1:C155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" zoomScale="92" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F154" sqref="F154"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="92" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B158" sqref="B158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1829,10 +1832,10 @@
         <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>291</v>
+        <v>449</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>291</v>
+        <v>450</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1840,10 +1843,10 @@
         <v>171</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1854,7 +1857,7 @@
         <v>286</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1865,7 +1868,7 @@
         <v>153</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1876,7 +1879,7 @@
         <v>48</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="68" x14ac:dyDescent="0.2">
@@ -1887,7 +1890,7 @@
         <v>287</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="119" x14ac:dyDescent="0.2">
@@ -1898,7 +1901,7 @@
         <v>42</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="119" x14ac:dyDescent="0.2">
@@ -1906,10 +1909,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1920,7 +1923,7 @@
         <v>288</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1942,7 +1945,7 @@
         <v>44</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1953,7 +1956,7 @@
         <v>172</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="85" x14ac:dyDescent="0.2">
@@ -1964,7 +1967,7 @@
         <v>218</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1975,7 +1978,7 @@
         <v>45</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1986,7 +1989,7 @@
         <v>46</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="85" x14ac:dyDescent="0.2">
@@ -1997,7 +2000,7 @@
         <v>50</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2019,7 +2022,7 @@
         <v>52</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2030,7 +2033,7 @@
         <v>53</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -2041,7 +2044,7 @@
         <v>54</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2052,7 +2055,7 @@
         <v>55</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -2063,7 +2066,7 @@
         <v>155</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2113,7 +2116,7 @@
         <v>59</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2124,7 +2127,7 @@
         <v>60</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2146,7 +2149,7 @@
         <v>62</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2168,7 +2171,7 @@
         <v>262</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -2179,7 +2182,7 @@
         <v>173</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -2201,7 +2204,7 @@
         <v>65</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -2212,7 +2215,7 @@
         <v>169</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2223,7 +2226,7 @@
         <v>66</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2234,7 +2237,7 @@
         <v>67</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2245,7 +2248,7 @@
         <v>69</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2256,7 +2259,7 @@
         <v>68</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2267,7 +2270,7 @@
         <v>70</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2278,7 +2281,7 @@
         <v>71</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="68" x14ac:dyDescent="0.2">
@@ -2289,7 +2292,7 @@
         <v>102</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -2300,7 +2303,7 @@
         <v>289</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2322,7 +2325,7 @@
         <v>141</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -2333,7 +2336,7 @@
         <v>290</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="68" x14ac:dyDescent="0.2">
@@ -2344,7 +2347,7 @@
         <v>104</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2366,7 +2369,7 @@
         <v>106</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -2377,7 +2380,7 @@
         <v>107</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -2388,7 +2391,7 @@
         <v>108</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2399,7 +2402,7 @@
         <v>109</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2410,7 +2413,7 @@
         <v>110</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="68" x14ac:dyDescent="0.2">
@@ -2421,7 +2424,7 @@
         <v>111</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="85" x14ac:dyDescent="0.2">
@@ -2432,7 +2435,7 @@
         <v>239</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -2443,7 +2446,7 @@
         <v>112</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2454,7 +2457,7 @@
         <v>113</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2465,7 +2468,7 @@
         <v>114</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="119" x14ac:dyDescent="0.2">
@@ -2476,7 +2479,7 @@
         <v>115</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="187" x14ac:dyDescent="0.2">
@@ -2487,7 +2490,7 @@
         <v>116</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -2498,7 +2501,7 @@
         <v>117</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2520,7 +2523,7 @@
         <v>266</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2575,7 +2578,7 @@
         <v>119</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="85" x14ac:dyDescent="0.2">
@@ -2586,7 +2589,7 @@
         <v>261</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -2597,7 +2600,7 @@
         <v>274</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -2608,7 +2611,7 @@
         <v>132</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -2619,7 +2622,7 @@
         <v>133</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -2630,7 +2633,7 @@
         <v>165</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -2641,7 +2644,7 @@
         <v>134</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2652,7 +2655,7 @@
         <v>135</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2663,7 +2666,7 @@
         <v>166</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2674,7 +2677,7 @@
         <v>138</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2718,7 +2721,7 @@
         <v>143</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2751,7 +2754,7 @@
         <v>151</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2762,7 +2765,7 @@
         <v>150</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2773,7 +2776,7 @@
         <v>168</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -2784,7 +2787,7 @@
         <v>260</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2795,7 +2798,7 @@
         <v>175</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2817,7 +2820,7 @@
         <v>178</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -2828,7 +2831,7 @@
         <v>263</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -2839,7 +2842,7 @@
         <v>173</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2850,7 +2853,7 @@
         <v>240</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2905,7 +2908,7 @@
         <v>200</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2916,7 +2919,7 @@
         <v>201</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2938,7 +2941,7 @@
         <v>212</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="102" x14ac:dyDescent="0.2">
@@ -2949,7 +2952,7 @@
         <v>215</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="85" x14ac:dyDescent="0.2">
@@ -2960,7 +2963,7 @@
         <v>213</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="68" x14ac:dyDescent="0.2">
@@ -2971,7 +2974,7 @@
         <v>214</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="102" x14ac:dyDescent="0.2">
@@ -2982,7 +2985,7 @@
         <v>216</v>
       </c>
       <c r="C107" s="5" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="85" x14ac:dyDescent="0.2">
@@ -2993,7 +2996,7 @@
         <v>217</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="85" x14ac:dyDescent="0.2">
@@ -3004,7 +3007,7 @@
         <v>219</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -3026,7 +3029,7 @@
         <v>238</v>
       </c>
       <c r="C111" s="5" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -3103,7 +3106,7 @@
         <v>248</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -3114,7 +3117,7 @@
         <v>249</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -3147,7 +3150,7 @@
         <v>248</v>
       </c>
       <c r="C122" s="5" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -3158,7 +3161,7 @@
         <v>256</v>
       </c>
       <c r="C123" s="5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -3169,7 +3172,7 @@
         <v>273</v>
       </c>
       <c r="C124" s="5" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="136" x14ac:dyDescent="0.2">
@@ -3180,7 +3183,7 @@
         <v>257</v>
       </c>
       <c r="C125" s="5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -3191,7 +3194,7 @@
         <v>285</v>
       </c>
       <c r="C126" s="5" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -3224,7 +3227,7 @@
         <v>280</v>
       </c>
       <c r="C129" s="5" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="153" x14ac:dyDescent="0.2">
@@ -3235,7 +3238,7 @@
         <v>281</v>
       </c>
       <c r="C130" s="5" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="119" x14ac:dyDescent="0.2">
@@ -3246,7 +3249,7 @@
         <v>282</v>
       </c>
       <c r="C131" s="5" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="153" x14ac:dyDescent="0.2">
@@ -3257,7 +3260,7 @@
         <v>283</v>
       </c>
       <c r="C132" s="5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -3268,249 +3271,249 @@
         <v>284</v>
       </c>
       <c r="C133" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C134" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C135" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C136" s="5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C137" s="5" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C138" s="5" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="139" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C139" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C140" s="5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C141" s="5" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C142" s="5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C143" s="5" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C144" s="5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C146" s="5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C147" s="5" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="148" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C148" s="5" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="149" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C149" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="150" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C150" s="5" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="151" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C151" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="152" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C152" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="153" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C153" s="5" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="154" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C154" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="155" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
     </row>
   </sheetData>
@@ -3796,16 +3799,16 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96E2A03F-E3AD-4163-99CA-F3F28F0C8F9F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a37677e5-1b95-4b15-ad17-c2245905d011"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="a37677e5-1b95-4b15-ad17-c2245905d011"/>
     <ds:schemaRef ds:uri="8c3b28d1-dd5b-4818-90bf-d163a72c8f0a"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
edits to publish app on Centroid account
</commit_message>
<xml_diff>
--- a/ges_health_study_app/text_dictionary.xlsx
+++ b/ges_health_study_app/text_dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uillinoisedu.sharepoint.com/sites/MarteniesLab2/Shared Documents/HELE Lab/projects/ges_health_study/data_analysis/ges_health_study_app/ges_health_study_app/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caitlinmothes/Desktop/ges_health_study_app/ges_health_study_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{271962A7-64A8-B944-AA4D-4D98F3015327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3BD903DD-CF80-AA41-99D0-A179FF7E0E59}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334FDF05-D8F5-A44D-99A8-7CEA274C31CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{8CCB3879-A5FF-D846-9F66-5161AE062B3F}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="16280" xr2:uid="{8CCB3879-A5FF-D846-9F66-5161AE062B3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1385,16 +1385,16 @@
     <t>&lt;b&gt;Cómo utilizar esta aplicación:&lt;/b&gt; Esta aplicación incluye herramientas para ayudar a los usuarios a comprender mejor la distribución de exposiciones ambientales y resultados de salud en Denver. El propósito de esta aplicación es documentar las tendencias en los factores sociales y ambientales que impactan la salud en los vecindarios de Denver, para que los residentes de la comunidad puedan aprender más sobre las condiciones que existen donde viven. Los datos disponibles en esta aplicación no deben utilizarse para hacer determinaciones sobre las causas específicas de la salud o enfermedades de cualquier residente que viva en Denver.</t>
   </si>
   <si>
-    <t>Lea este sitio en español: &lt;a href='https://geshealthstudy.shinyapps.io/ges_health_study_app_espanol'&gt; Mapas interactivos del Estudio de salud comunitaria del GES&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>Lea este sitio en inglés: &lt;a href='https://geshealthstudy.shinyapps.io/ges_health_study_app_english'&gt; Mapas interactivos del Estudio de salud comunitaria del GES&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>&lt;strong&gt;Recommended Citation: &lt;/strong&gt; Estudio de Nuestros Vecinos para Investigar los Riesgos y Nuestra Salud (ENVIRONS). February 2025. GES Community Health Study Interactive Maps. Fort Collins, CO.</t>
   </si>
   <si>
     <t>&lt;strong&gt;Cita recomendada: &lt;/strong&gt; Estudio de Nuestros Vecinos para Investigar los Riesgos y Nuestra Salud (ENVIRONS). Febrero de 2025. Mapas Interactivos del Estudio de Salud Comunitaria GES. Fort Collins, CO.</t>
+  </si>
+  <si>
+    <t>Lea este sitio en inglés: &lt;a href='https://geocentroid.shinyapps.io/ges_health_study_app_english/'&gt; Mapas interactivos del Estudio de salud comunitaria del GES&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Lea este sitio en español: &lt;a href='https://geocentroid.shinyapps.io/ges_health_study_app_espanol/'&gt; Mapas interactivos del Estudio de salud comunitaria del GES&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -1804,14 +1804,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{548E5ED1-4340-C04D-8029-23B2D57DC5C7}">
   <dimension ref="A1:C155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="92" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B158" sqref="B158"/>
+    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="86.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="99.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="97.5" style="4" customWidth="1"/>
     <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
@@ -1827,15 +1827,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -3510,10 +3510,10 @@
         <v>446</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
   </sheetData>
@@ -3526,15 +3526,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="a37677e5-1b95-4b15-ad17-c2245905d011" xsi:nil="true"/>
@@ -3543,6 +3534,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3789,14 +3789,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9E24F5B-1456-48CF-91D3-C32867BD6122}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96E2A03F-E3AD-4163-99CA-F3F28F0C8F9F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -3809,6 +3801,14 @@
     <ds:schemaRef ds:uri="8c3b28d1-dd5b-4818-90bf-d163a72c8f0a"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9E24F5B-1456-48CF-91D3-C32867BD6122}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>